<commit_message>
Revisione finale finale finale
</commit_message>
<xml_diff>
--- a/BOP_realistic_instance_v2.xlsx
+++ b/BOP_realistic_instance_v2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emapi\PycharmProjects\wm-bilevel-opt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8417B9FF-E0EA-45B1-BBFF-5C2245891EA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{142C0CBC-5D44-4B9D-9C4F-256A8ED388D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8196" yWindow="1356" windowWidth="17280" windowHeight="8880" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="client" sheetId="1" r:id="rId1"/>
@@ -496,12 +496,18 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -516,7 +522,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -525,6 +531,7 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1854,7 +1861,7 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1925,24 +1932,24 @@
         <v>30.547945205479451</v>
       </c>
       <c r="H2" s="1">
-        <f>F2/3</f>
-        <v>3716.6666666666665</v>
+        <f>F2/5</f>
+        <v>2230</v>
       </c>
       <c r="I2" s="1">
         <f t="shared" ref="I2:I11" si="1">J2*0.7</f>
-        <v>7.1278538812785381</v>
+        <v>4.2767123287671236</v>
       </c>
       <c r="J2" s="1">
         <f>H2/365</f>
-        <v>10.182648401826484</v>
+        <v>6.1095890410958908</v>
       </c>
       <c r="K2" s="1">
         <f t="shared" ref="K2:K11" si="2">J2*1.3</f>
-        <v>13.237442922374429</v>
+        <v>7.9424657534246581</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
+      <c r="A3" s="4">
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -1965,20 +1972,20 @@
         <v>41.095890410958901</v>
       </c>
       <c r="H3" s="1">
-        <f t="shared" ref="H3:H11" si="3">F3/3</f>
-        <v>5000</v>
+        <f t="shared" ref="H3:H11" si="3">F3/5</f>
+        <v>3000</v>
       </c>
       <c r="I3" s="1">
         <f t="shared" si="1"/>
-        <v>9.5890410958904102</v>
+        <v>5.7534246575342465</v>
       </c>
       <c r="J3" s="1">
         <f t="shared" ref="J3:J11" si="4">H3/365</f>
-        <v>13.698630136986301</v>
+        <v>8.2191780821917817</v>
       </c>
       <c r="K3" s="1">
         <f t="shared" si="2"/>
-        <v>17.808219178082194</v>
+        <v>10.684931506849317</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
@@ -2006,19 +2013,19 @@
       </c>
       <c r="H4" s="1">
         <f t="shared" si="3"/>
-        <v>23333.333333333332</v>
+        <v>14000</v>
       </c>
       <c r="I4" s="1">
         <f t="shared" si="1"/>
-        <v>44.74885844748858</v>
+        <v>26.849315068493148</v>
       </c>
       <c r="J4" s="1">
         <f t="shared" si="4"/>
-        <v>63.926940639269404</v>
+        <v>38.356164383561641</v>
       </c>
       <c r="K4" s="1">
         <f t="shared" si="2"/>
-        <v>83.105022831050235</v>
+        <v>49.863013698630134</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
@@ -2046,19 +2053,19 @@
       </c>
       <c r="H5" s="1">
         <f t="shared" si="3"/>
-        <v>20000</v>
+        <v>12000</v>
       </c>
       <c r="I5" s="1">
         <f t="shared" si="1"/>
-        <v>38.356164383561641</v>
+        <v>23.013698630136986</v>
       </c>
       <c r="J5" s="1">
         <f t="shared" si="4"/>
-        <v>54.794520547945204</v>
+        <v>32.876712328767127</v>
       </c>
       <c r="K5" s="1">
         <f t="shared" si="2"/>
-        <v>71.232876712328775</v>
+        <v>42.739726027397268</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
@@ -2086,23 +2093,23 @@
       </c>
       <c r="H6" s="1">
         <f t="shared" si="3"/>
-        <v>17000</v>
+        <v>10200</v>
       </c>
       <c r="I6" s="1">
         <f t="shared" si="1"/>
-        <v>32.602739726027394</v>
+        <v>19.561643835616437</v>
       </c>
       <c r="J6" s="1">
         <f t="shared" si="4"/>
-        <v>46.575342465753423</v>
+        <v>27.945205479452056</v>
       </c>
       <c r="K6" s="1">
         <f t="shared" si="2"/>
-        <v>60.547945205479451</v>
+        <v>36.328767123287676</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="1">
+      <c r="A7" s="4">
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -2126,23 +2133,23 @@
       </c>
       <c r="H7" s="1">
         <f t="shared" si="3"/>
-        <v>28000</v>
+        <v>16800</v>
       </c>
       <c r="I7" s="1">
         <f t="shared" si="1"/>
-        <v>53.698630136986296</v>
+        <v>32.219178082191782</v>
       </c>
       <c r="J7" s="1">
         <f t="shared" si="4"/>
-        <v>76.712328767123282</v>
+        <v>46.027397260273972</v>
       </c>
       <c r="K7" s="1">
         <f t="shared" si="2"/>
-        <v>99.726027397260268</v>
+        <v>59.835616438356162</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="1">
+      <c r="A8" s="4">
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -2166,19 +2173,19 @@
       </c>
       <c r="H8" s="1">
         <f t="shared" si="3"/>
-        <v>15000</v>
+        <v>9000</v>
       </c>
       <c r="I8" s="1">
         <f t="shared" si="1"/>
-        <v>28.767123287671229</v>
+        <v>17.260273972602739</v>
       </c>
       <c r="J8" s="1">
         <f t="shared" si="4"/>
-        <v>41.095890410958901</v>
+        <v>24.657534246575342</v>
       </c>
       <c r="K8" s="1">
         <f t="shared" si="2"/>
-        <v>53.42465753424657</v>
+        <v>32.054794520547944</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
@@ -2206,23 +2213,23 @@
       </c>
       <c r="H9" s="1">
         <f t="shared" si="3"/>
-        <v>31000</v>
+        <v>18600</v>
       </c>
       <c r="I9" s="1">
         <f t="shared" si="1"/>
-        <v>59.452054794520542</v>
+        <v>35.671232876712324</v>
       </c>
       <c r="J9" s="1">
         <f t="shared" si="4"/>
-        <v>84.93150684931507</v>
+        <v>50.958904109589042</v>
       </c>
       <c r="K9" s="1">
         <f t="shared" si="2"/>
-        <v>110.41095890410959</v>
+        <v>66.246575342465761</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="1">
+      <c r="A10" s="4">
         <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -2246,23 +2253,23 @@
       </c>
       <c r="H10" s="1">
         <f t="shared" si="3"/>
-        <v>26166.666666666668</v>
+        <v>15700</v>
       </c>
       <c r="I10" s="1">
         <f t="shared" si="1"/>
-        <v>50.182648401826484</v>
+        <v>30.109589041095887</v>
       </c>
       <c r="J10" s="1">
         <f t="shared" si="4"/>
-        <v>71.689497716894977</v>
+        <v>43.013698630136986</v>
       </c>
       <c r="K10" s="1">
         <f t="shared" si="2"/>
-        <v>93.196347031963469</v>
+        <v>55.917808219178085</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="1">
+      <c r="A11" s="4">
         <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -2286,19 +2293,19 @@
       </c>
       <c r="H11" s="1">
         <f t="shared" si="3"/>
-        <v>32000</v>
+        <v>19200</v>
       </c>
       <c r="I11" s="1">
         <f t="shared" si="1"/>
-        <v>61.36986301369862</v>
+        <v>36.821917808219176</v>
       </c>
       <c r="J11" s="1">
         <f t="shared" si="4"/>
-        <v>87.671232876712324</v>
+        <v>52.602739726027394</v>
       </c>
       <c r="K11" s="1">
         <f t="shared" si="2"/>
-        <v>113.97260273972603</v>
+        <v>68.38356164383562</v>
       </c>
     </row>
   </sheetData>

</xml_diff>